<commit_message>
Updated after more work
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IASTATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41793F55-251F-416D-8CD2-62AF0E1976DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FAB06-7E97-4788-AF89-0AF33D7EFA6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1022,7 +1022,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>179</c:v>
+                  <c:v>179.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>105</c:v>
@@ -1037,7 +1037,7 @@
                   <c:v>180.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>135</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,7 +1566,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0</c:v>
@@ -2306,7 +2306,7 @@
                   <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>0</c:v>
@@ -3075,7 +3075,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>179</c:v>
+                  <c:v>179.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3705,7 +3705,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>135</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4321,7 +4321,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6146,7 +6146,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9635,7 +9635,7 @@
   <dimension ref="A1:AG122"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+      <selection activeCell="G103" sqref="G103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9694,7 +9694,7 @@
       </c>
       <c r="B2" s="5">
         <f>SUM(B4:B166)</f>
-        <v>179</v>
+        <v>179.5</v>
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
@@ -9714,11 +9714,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>953.5</v>
+        <v>956</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12864,7 +12864,7 @@
         <v>23</v>
       </c>
       <c r="B102" s="15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C102" s="15">
         <v>0</v>
@@ -12879,11 +12879,11 @@
         <v>2</v>
       </c>
       <c r="G102" s="15">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H102" s="1">
         <f t="shared" ref="H102:H107" si="11">SUM(B102:G102)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="I102" s="24">
         <v>99</v>
@@ -13034,7 +13034,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <f>SUM(H102:H108)</f>
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>

</xml_diff>

<commit_message>
Today's initial work log
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FAB06-7E97-4788-AF89-0AF33D7EFA6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A23D82-EFD4-4284-B407-E396DB3B4891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -1025,19 +1025,19 @@
                   <c:v>179.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>105.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136</c:v>
+                  <c:v>136.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>180.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>137</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1569,7 +1569,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>0</c:v>
@@ -2309,7 +2309,7 @@
                   <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>0</c:v>
@@ -3201,7 +3201,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>105</c:v>
+                  <c:v>105.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3453,7 +3453,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>136</c:v>
+                  <c:v>136.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3705,7 +3705,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>137</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4323,6 +4323,9 @@
                 <c:pt idx="98">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4688,6 +4691,9 @@
                 <c:pt idx="98">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5053,6 +5059,9 @@
                 <c:pt idx="98">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5418,6 +5427,9 @@
                 <c:pt idx="98">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5783,6 +5795,9 @@
                 <c:pt idx="98">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="99">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6147,6 +6162,9 @@
                 </c:pt>
                 <c:pt idx="98">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9634,8 +9652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G103" sqref="G103"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9698,7 +9716,7 @@
       </c>
       <c r="C2" s="6">
         <f>SUM(C4:C150)</f>
-        <v>105</v>
+        <v>105.5</v>
       </c>
       <c r="D2" s="7">
         <f>SUM(D4:D150)</f>
@@ -9706,7 +9724,7 @@
       </c>
       <c r="E2" s="8">
         <f>SUM(E4:E150)</f>
-        <v>136</v>
+        <v>136.5</v>
       </c>
       <c r="F2" s="9">
         <f>SUM(F4:F150)</f>
@@ -9714,11 +9732,11 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(G4:G150)</f>
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H2" s="3">
         <f>SUM(B2:G2)</f>
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="I2" s="25"/>
       <c r="J2" s="28"/>
@@ -12897,15 +12915,27 @@
         <f>SUM(H95:H101)</f>
         <v>76.5</v>
       </c>
-      <c r="B103" s="15"/>
-      <c r="C103" s="15"/>
-      <c r="D103" s="15"/>
-      <c r="E103" s="15"/>
-      <c r="F103" s="15"/>
-      <c r="G103" s="15"/>
+      <c r="B103" s="15">
+        <v>0</v>
+      </c>
+      <c r="C103" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="D103" s="15">
+        <v>0</v>
+      </c>
+      <c r="E103" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="F103" s="15">
+        <v>0</v>
+      </c>
+      <c r="G103" s="15">
+        <v>2</v>
+      </c>
       <c r="H103" s="1">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I103" s="24">
         <v>100</v>
@@ -13034,7 +13064,7 @@
     <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="14">
         <f>SUM(H102:H108)</f>
-        <v>7.5</v>
+        <v>10.5</v>
       </c>
       <c r="B110" s="17"/>
       <c r="C110" s="17"/>

</xml_diff>

<commit_message>
Finalization of work exc
</commit_message>
<xml_diff>
--- a/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
+++ b/CollegeSemesterWork/TimeSpentWorkingSemester6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt8\repo\mghoskins-Data\CollegeSemesterWork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9EFABC-29D7-4DA6-9508-5A48F774D353}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535F87BE-1CE3-4B3B-8FAC-B2E2EFE8984A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{82375D23-D698-41CA-AAE3-ABC009559D4F}"/>
   </bookViews>
@@ -4329,6 +4329,9 @@
                 <c:pt idx="100">
                   <c:v>0.5</c:v>
                 </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4700,6 +4703,9 @@
                 <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5071,6 +5077,9 @@
                 <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5442,6 +5451,9 @@
                 <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5813,6 +5825,9 @@
                 <c:pt idx="100">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6183,6 +6198,9 @@
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9670,8 +9688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE33D67F-891D-4EAD-9F40-3D033E7F434D}">
   <dimension ref="A1:AG122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9838,8 +9856,8 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
-        <f>AVERAGE(H4:H101)</f>
-        <v>9.6785714285714288</v>
+        <f>AVERAGE(H4:H105)</f>
+        <v>9.4558823529411757</v>
       </c>
       <c r="B6" s="15">
         <v>0.25</v>
@@ -12993,12 +13011,24 @@
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B105" s="15"/>
-      <c r="C105" s="15"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="15"/>
+      <c r="B105" s="15">
+        <v>0</v>
+      </c>
+      <c r="C105" s="15">
+        <v>0</v>
+      </c>
+      <c r="D105" s="15">
+        <v>0</v>
+      </c>
+      <c r="E105" s="15">
+        <v>0</v>
+      </c>
+      <c r="F105" s="15">
+        <v>0</v>
+      </c>
+      <c r="G105" s="15">
+        <v>0</v>
+      </c>
       <c r="H105" s="1">
         <f t="shared" si="11"/>
         <v>0</v>

</xml_diff>